<commit_message>
Se puede descargar el exel ahora mismo!
</commit_message>
<xml_diff>
--- a/ventas.xlsx
+++ b/ventas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45844</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Poker x30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Unitario</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>